<commit_message>
Forgot to save the excel file.
</commit_message>
<xml_diff>
--- a/transformer_results_full-grid.xlsx
+++ b/transformer_results_full-grid.xlsx
@@ -2233,10 +2233,10 @@
     <t xml:space="preserve">transformer_model_20231208195003</t>
   </si>
   <si>
+    <t xml:space="preserve">transformer_model_20231210194546</t>
+  </si>
+  <si>
     <t xml:space="preserve">transformer_model_20231208180627</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transformer_model_20231210194546</t>
   </si>
 </sst>
 </file>
@@ -2376,10 +2376,10 @@
   <dimension ref="A1:J730"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.36"/>
@@ -2388,7 +2388,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.91"/>
   </cols>
   <sheetData>
@@ -25693,16 +25693,16 @@
         <v>736</v>
       </c>
       <c r="C729" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D729" s="0" t="n">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E729" s="0" t="n">
         <v>16</v>
       </c>
       <c r="F729" s="0" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="G729" s="0" t="n">
         <v>2</v>
@@ -25711,7 +25711,7 @@
         <v>16</v>
       </c>
       <c r="J729" s="0" t="n">
-        <v>0.3376285135746</v>
+        <v>0.339643150568008</v>
       </c>
     </row>
     <row r="730" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25722,16 +25722,16 @@
         <v>737</v>
       </c>
       <c r="C730" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D730" s="0" t="n">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E730" s="0" t="n">
         <v>16</v>
       </c>
       <c r="F730" s="0" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="G730" s="0" t="n">
         <v>2</v>
@@ -25740,7 +25740,7 @@
         <v>16</v>
       </c>
       <c r="J730" s="0" t="n">
-        <v>0.339643150568008</v>
+        <v>0.3376285135746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>